<commit_message>
23.187 대응 (txt 제외)
</commit_message>
<xml_diff>
--- a/Mod_Korean/Lang/KR/Dialog/Drama/fairy_nanasu.xlsx
+++ b/Mod_Korean/Lang/KR/Dialog/Drama/fairy_nanasu.xlsx
@@ -145,7 +145,7 @@
         <charset val="129"/>
       </rPr>
       <t xml:space="preserve">… 들어줄 거야~?
-스펙윙을 방문하는 모험가들 사이에, 어떤 네피아에 터무니없는 보물이 잠들어 있다는 소문이 파다해~ 그 보물이라는 게 말이야, 안에 뭘 넣든 간에 가볍게 만들어 주는 신비한 가방이래!</t>
+스펙윙을 방문하는 모험가들 사이에, 어떤 네피아에 터무니없는 보물이 잠들어 있다는 소문이 파다해~ 그리고 그 보물이라는 게 말이야, 안에 뭘 넣든 간에 가볍게 만들어 주는 신비한 가방이래!</t>
     </r>
   </si>
   <si>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">You know how I’m not very strong, right? My pack always ends up too heavy, and sometimes I feel like crying in the middle of a trip. But if I had that bag, I could go farther than ever before! I could meet more people, and every adventure would become even more fun.</t>
   </si>
   <si>
-    <t xml:space="preserve">봐봐, 나는 약골이잖아? 항상 짐이 무거워서 모험을 하다가 눈물을 펑펑 쏟는단 말이지~ 만약에 그 가방이 있다면, 좀 더 멀리까지 가볼 수 있지 않을까 하는 거야~ 좀 더 다양한 사람들과 만나서, 더 더 즐거운 모험을 할 수 있게 되겠지~</t>
+    <t xml:space="preserve">봐봐, 나는 약골이잖아? 항상 짐이 무거워서 모험을 하다가 눈물을 펑펑 쏟는단 말이지~ 만약 그 가방이 있다면, 좀 더 멀리까지 가볼 수 있지 않을까 하는 거야~ 좀 더 다양한 사람들과 만나서, 더 더 즐거운 모험을 할 수 있게 되겠지~</t>
   </si>
   <si>
     <t xml:space="preserve">でもねぇ…「帰らずの森」は、ボク一人で探索するにはちょっと怖い場所なんだ～。だからさ、冒険者さん…ボクと一緒に行ってくれないかな～？
@@ -335,7 +335,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">오오~ 해냈구나, 모험가님! 진짜로, 진짜로 있었어! </t>
+      <t xml:space="preserve">오오~ 우리가 해냈구나, 모험가님! 진짜로, 진짜로 있었어! </t>
     </r>
     <r>
       <rPr>
@@ -440,7 +440,7 @@
         <family val="0"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve">… 뭔가 날개가 찌릿찌릿 한데?</t>
+      <t xml:space="preserve">… 왠지 날개가 찌릿찌릿한데?</t>
     </r>
   </si>
   <si>
@@ -572,7 +572,7 @@
     <t xml:space="preserve">Aww, come on, Poina! Killing them right away would be boring! Where’s the fun in that?</t>
   </si>
   <si>
-    <t xml:space="preserve">아니, 들어 봐 포이나, 갑자기 죽여버리면 재미가 없지 않아?</t>
+    <t xml:space="preserve">아니, 들어 봐 포이나, 갑자기 죽여버리는 건 재미가 없지 않아?</t>
   </si>
   <si>
     <t xml:space="preserve">ねえナナス？　アタシ、この鞄なんてどうでもいいんだよねぇ。本当はただ…アンタの困った顔が見たかっただけ。泣き虫ナナスが「やめてよぉ～」って言うの、最高に楽しいんだもん。だからねぇ……返せ？ いやだねぇ！奪いたいなら、力ずくでどうぞって感じぃ！ほらほら、早くかかってきなよ、今日もビリビリして焼きナスにしてあげるからさぁ！</t>
@@ -707,7 +707,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">바보냐고</t>
+      <t xml:space="preserve">멍청이가</t>
     </r>
     <r>
       <rPr>
@@ -1164,9 +1164,9 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="bottomLeft" activeCell="L56" activeCellId="0" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1487,7 +1487,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="67.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I41" s="1" t="n">
         <v>10</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="1" t="n">
         <v>12</v>
       </c>

</xml_diff>